<commit_message>
upload results for Sweden
</commit_message>
<xml_diff>
--- a/1D-model/input/Backa/Backa daily increase and removal amount.xlsx
+++ b/1D-model/input/Backa/Backa daily increase and removal amount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\AAFC\Project 10_STM\2_method\STM-and-1D-model\1D-model\input\Backa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE850DD7-C451-4286-8E9B-59601830B017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536BF5DE-DE27-4F69-897A-A2AA56BDE109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11110" yWindow="0" windowWidth="11380" windowHeight="13370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4910" yWindow="3550" windowWidth="9540" windowHeight="11450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H_level" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>doy     level</t>
   </si>
@@ -68,12 +68,6 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>Mar 31 - Apr 1</t>
-  </si>
-  <si>
-    <t>Jan 23 - Jan 25</t>
-  </si>
-  <si>
     <t>100-101</t>
   </si>
   <si>
@@ -84,6 +78,30 @@
   </si>
   <si>
     <t>Total removal</t>
+  </si>
+  <si>
+    <t>Estimated days</t>
+  </si>
+  <si>
+    <t>Apr 10 - Apr 11</t>
+  </si>
+  <si>
+    <t>Aug 18 - Aug 26</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>May 16, 2020 - Aug 17, 2020</t>
+  </si>
+  <si>
+    <t>Aug 18, 2020 - Dec 31, 2020</t>
+  </si>
+  <si>
+    <t>rearranged days (because the start date is May 16</t>
+  </si>
+  <si>
+    <t>Jan 1, 2021 -  May 16, 2021</t>
   </si>
 </sst>
 </file>
@@ -567,10 +585,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -708,10 +727,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>H_level!$A$2:$A$128</c:f>
+              <c:f>H_level!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="127"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -741,10 +760,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>H_level!$B$2:$B$128</c:f>
+              <c:f>H_level!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="127"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1526,13 +1545,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>339725</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>155575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>34925</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>136525</xdr:rowOff>
@@ -1860,204 +1879,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.36328125" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.36328125" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
+        <v>44197</v>
+      </c>
+      <c r="C2">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <f>SLOPE(B2:B4,A2:A4)</f>
+      <c r="F2">
+        <f>SLOPE(C2:C4,A2:A4)</f>
         <v>1.0190993164455167E-2</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>100</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <f>F3</f>
+        <v>1.0083171311298336E-2</v>
+      </c>
+      <c r="J2">
+        <f>A7-J4</f>
+        <v>94</v>
+      </c>
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>61</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
+        <v>44257</v>
+      </c>
+      <c r="C3">
         <v>3.67</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3">
-        <f>SLOPE(B5:B7,A5:A7)</f>
+      <c r="F3">
+        <f>SLOPE(C5:C7,A5:A7)</f>
         <v>1.0083171311298336E-2</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>130</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <f>B4-B5</f>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <f>F4</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J3">
+        <f>A9-J4-J2 +366-A9</f>
+        <v>136</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <f>C4-C5</f>
         <v>2.5</v>
       </c>
-      <c r="I3">
-        <f>H3*D$8+D$9*2</f>
+      <c r="N3">
+        <f>M3*F$8+F$9*2</f>
         <v>2522.4061802502665</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>100</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
+        <v>44296</v>
+      </c>
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4">
-        <f>SLOPE(B8:B9,A8:A9)</f>
+      <c r="F4">
+        <f>SLOPE(C8:C9,A8:A9)</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>65</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4">
-        <f>B7-B8</f>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4">
+        <f>F2</f>
+        <v>1.0190993164455167E-2</v>
+      </c>
+      <c r="J4">
+        <v>136</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4">
+        <f>C7-C8</f>
         <v>1.67</v>
       </c>
-      <c r="I4">
-        <f>H4*D$8+D$9*1</f>
+      <c r="N4">
+        <f>M4*F$8+F$9*1</f>
         <v>1681.2030901251333</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>101</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
+        <v>44297</v>
+      </c>
+      <c r="C5">
         <v>1.5</v>
       </c>
+      <c r="J5">
+        <f>SUM(J2:J4)</f>
+        <v>366</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>128</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
+        <v>44324</v>
+      </c>
+      <c r="C6">
         <v>1.77</v>
       </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6">
-        <f>SUM(I3:I4)</f>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6">
+        <f>SUM(N3:N4)</f>
         <v>4203.6092703754002</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>230</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
+        <v>44060</v>
+      </c>
+      <c r="C7">
         <v>2.8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="D7">
-        <f>SUMPRODUCT(D2:D4,E2:E4)/SUM(E2:E4)</f>
+      <c r="F7">
+        <f>SUMPRODUCT(F2:F4,G2:G4)/SUM(G2:G4)</f>
         <v>1.1203090125133222E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>238</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
+        <v>44068</v>
+      </c>
+      <c r="C8">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>302</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
+        <v>44132</v>
+      </c>
+      <c r="C9">
         <v>2.09</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1">
-        <f>D7*D8</f>
+      <c r="F9" s="1">
+        <f>F7*F8</f>
         <v>11.203090125133222</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2">
-        <f>D7*D8*366</f>
+      <c r="F10" s="2">
+        <f>F7*F8*366</f>
         <v>4100.3309857987597</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>